<commit_message>
added TC5.1 & TC 5.2 (done some fixes)
</commit_message>
<xml_diff>
--- a/doc/TA.Final.TestCases.DoroshenkoDenis.xlsx
+++ b/doc/TA.Final.TestCases.DoroshenkoDenis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\NetcrackerLearningCenter\finalPractice\cucumber-selenium\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FE60368-2C27-4C1C-8C2A-E2E151CBE1E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111AD3F9-21AB-4142-B363-415E9880B5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-8010" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="193">
   <si>
     <t>TC_ID</t>
   </si>
@@ -666,6 +666,9 @@
   </si>
   <si>
     <t>Username:  random alphanumeric string (length =&gt; 6 and &lt;= 50); Password - "password1="; Confirm password - same with Password; e-mail: Username + "@testmail.com"</t>
+  </si>
+  <si>
+    <t>2.  Point the mouse at Infrastructure Orders and click</t>
   </si>
 </sst>
 </file>
@@ -1547,6 +1550,15 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1556,6 +1568,33 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1565,13 +1604,88 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1583,49 +1697,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1633,75 +1705,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="43" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2047,8 +2050,8 @@
   </sheetPr>
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C100" sqref="C100"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2079,12 +2082,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="87" t="s">
+      <c r="A2" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="88"/>
-      <c r="C2" s="88"/>
-      <c r="D2" s="89"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="78"/>
       <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
@@ -2093,14 +2096,14 @@
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="103" t="s">
+      <c r="B3" s="94" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="103"/>
-      <c r="D3" s="104"/>
+      <c r="C3" s="94"/>
+      <c r="D3" s="95"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="105" t="s">
+      <c r="A4" s="96" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="79" t="s">
@@ -2109,66 +2112,66 @@
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="106" t="s">
+      <c r="D4" s="97" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="105"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="79"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="106"/>
+      <c r="D5" s="97"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="105"/>
+      <c r="A6" s="96"/>
       <c r="B6" s="79"/>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="106"/>
+      <c r="D6" s="97"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="105"/>
+      <c r="A7" s="96"/>
       <c r="B7" s="79"/>
       <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="106"/>
+      <c r="D7" s="97"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="105"/>
+      <c r="A8" s="96"/>
       <c r="B8" s="79"/>
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="106"/>
+      <c r="D8" s="97"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="105"/>
+      <c r="A9" s="96"/>
       <c r="B9" s="79"/>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="106"/>
+      <c r="D9" s="97"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="105"/>
+      <c r="A10" s="96"/>
       <c r="B10" s="79"/>
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="106"/>
+      <c r="D10" s="97"/>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="105"/>
+      <c r="A11" s="96"/>
       <c r="B11" s="79"/>
       <c r="C11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="106"/>
+      <c r="D11" s="97"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
@@ -2202,62 +2205,62 @@
       <c r="A14" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="63"/>
+      <c r="C14" s="74"/>
+      <c r="D14" s="75"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="100" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="76" t="s">
+      <c r="B15" s="64" t="s">
         <v>169</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="67" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="74"/>
-      <c r="B16" s="77"/>
+      <c r="A16" s="101"/>
+      <c r="B16" s="65"/>
       <c r="C16" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="D16" s="65"/>
+      <c r="D16" s="68"/>
     </row>
     <row r="17" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="75"/>
-      <c r="B17" s="78"/>
+      <c r="A17" s="102"/>
+      <c r="B17" s="103"/>
       <c r="C17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="66"/>
+      <c r="D17" s="107"/>
     </row>
     <row r="18" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
+      <c r="C18" s="74"/>
+      <c r="D18" s="75"/>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="67" t="s">
+      <c r="A19" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="69"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="106"/>
     </row>
     <row r="20" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="93" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="79" t="s">
@@ -2266,17 +2269,17 @@
       <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="64" t="s">
+      <c r="D20" s="67" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="70"/>
+      <c r="A21" s="93"/>
       <c r="B21" s="79"/>
       <c r="C21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="65"/>
+      <c r="D21" s="68"/>
     </row>
     <row r="22" spans="1:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="54" t="s">
@@ -2288,28 +2291,28 @@
       <c r="C22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="66"/>
+      <c r="D22" s="107"/>
     </row>
     <row r="23" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="73" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="63"/>
+      <c r="C23" s="74"/>
+      <c r="D23" s="75"/>
     </row>
     <row r="24" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="69"/>
+      <c r="B24" s="105"/>
+      <c r="C24" s="105"/>
+      <c r="D24" s="106"/>
     </row>
     <row r="25" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="70" t="s">
+      <c r="A25" s="93" t="s">
         <v>61</v>
       </c>
       <c r="B25" s="79" t="s">
@@ -2318,17 +2321,17 @@
       <c r="C25" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D25" s="64" t="s">
+      <c r="D25" s="67" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="70"/>
+      <c r="A26" s="93"/>
       <c r="B26" s="79"/>
       <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="65"/>
+      <c r="D26" s="68"/>
     </row>
     <row r="27" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="56" t="s">
@@ -2340,7 +2343,7 @@
       <c r="C27" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="65"/>
+      <c r="D27" s="68"/>
     </row>
     <row r="28" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="55" t="s">
@@ -2352,7 +2355,7 @@
       <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="65"/>
+      <c r="D28" s="68"/>
     </row>
     <row r="29" spans="1:4" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="57" t="s">
@@ -2364,69 +2367,69 @@
       <c r="C29" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="66"/>
+      <c r="D29" s="107"/>
     </row>
     <row r="30" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="61" t="s">
+      <c r="B30" s="73" t="s">
         <v>135</v>
       </c>
-      <c r="C30" s="62"/>
-      <c r="D30" s="63"/>
+      <c r="C30" s="74"/>
+      <c r="D30" s="75"/>
     </row>
     <row r="31" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="80" t="s">
+      <c r="A31" s="70" t="s">
         <v>172</v>
       </c>
-      <c r="B31" s="81"/>
-      <c r="C31" s="81"/>
-      <c r="D31" s="82"/>
+      <c r="B31" s="71"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="72"/>
     </row>
     <row r="32" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="85" t="s">
+      <c r="A32" s="108" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="76" t="s">
+      <c r="B32" s="64" t="s">
         <v>84</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="64" t="s">
+      <c r="D32" s="67" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="86"/>
-      <c r="B33" s="84"/>
+      <c r="A33" s="109"/>
+      <c r="B33" s="66"/>
       <c r="C33" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="83"/>
+      <c r="D33" s="69"/>
     </row>
     <row r="34" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="85" t="s">
+      <c r="A34" s="108" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="76" t="s">
+      <c r="B34" s="64" t="s">
         <v>85</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="64" t="s">
+      <c r="D34" s="67" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="86"/>
-      <c r="B35" s="84"/>
+      <c r="A35" s="109"/>
+      <c r="B35" s="66"/>
       <c r="C35" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="D35" s="83"/>
+        <v>192</v>
+      </c>
+      <c r="D35" s="69"/>
     </row>
     <row r="36" spans="1:4" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
@@ -2446,13 +2449,13 @@
       <c r="A37" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="B37" s="76" t="s">
+      <c r="B37" s="64" t="s">
         <v>117</v>
       </c>
       <c r="C37" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="D37" s="64" t="s">
+      <c r="D37" s="67" t="s">
         <v>110</v>
       </c>
     </row>
@@ -2460,51 +2463,51 @@
       <c r="A38" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B38" s="77"/>
+      <c r="B38" s="65"/>
       <c r="C38" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="D38" s="65"/>
+      <c r="D38" s="68"/>
     </row>
     <row r="39" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="B39" s="77"/>
+      <c r="B39" s="65"/>
       <c r="C39" s="27" t="s">
         <v>120</v>
       </c>
-      <c r="D39" s="65"/>
+      <c r="D39" s="68"/>
     </row>
     <row r="40" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
         <v>118</v>
       </c>
-      <c r="B40" s="84"/>
+      <c r="B40" s="66"/>
       <c r="C40" s="27" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="83"/>
+      <c r="D40" s="69"/>
     </row>
     <row r="41" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="80" t="s">
+      <c r="A41" s="70" t="s">
         <v>127</v>
       </c>
-      <c r="B41" s="81"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="82"/>
+      <c r="B41" s="71"/>
+      <c r="C41" s="71"/>
+      <c r="D41" s="72"/>
     </row>
     <row r="42" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="76" t="s">
+      <c r="B42" s="64" t="s">
         <v>165</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="D42" s="64" t="s">
+      <c r="D42" s="67" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2512,21 +2515,21 @@
       <c r="A43" s="26" t="s">
         <v>164</v>
       </c>
-      <c r="B43" s="77"/>
+      <c r="B43" s="65"/>
       <c r="C43" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D43" s="65"/>
+      <c r="D43" s="68"/>
     </row>
     <row r="44" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
         <v>163</v>
       </c>
-      <c r="B44" s="84"/>
+      <c r="B44" s="66"/>
       <c r="C44" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="D44" s="83"/>
+      <c r="D44" s="69"/>
     </row>
     <row r="45" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
@@ -2560,19 +2563,19 @@
       <c r="A47" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="61" t="s">
+      <c r="B47" s="73" t="s">
         <v>136</v>
       </c>
-      <c r="C47" s="62"/>
-      <c r="D47" s="63"/>
+      <c r="C47" s="74"/>
+      <c r="D47" s="75"/>
     </row>
     <row r="48" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="80" t="s">
+      <c r="A48" s="70" t="s">
         <v>173</v>
       </c>
-      <c r="B48" s="81"/>
-      <c r="C48" s="81"/>
-      <c r="D48" s="82"/>
+      <c r="B48" s="71"/>
+      <c r="C48" s="71"/>
+      <c r="D48" s="72"/>
     </row>
     <row r="49" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
@@ -2646,19 +2649,19 @@
       <c r="A54" s="21" t="s">
         <v>143</v>
       </c>
-      <c r="B54" s="61" t="s">
+      <c r="B54" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="C54" s="62"/>
-      <c r="D54" s="63"/>
+      <c r="C54" s="74"/>
+      <c r="D54" s="75"/>
     </row>
     <row r="55" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="80" t="s">
+      <c r="A55" s="70" t="s">
         <v>175</v>
       </c>
-      <c r="B55" s="81"/>
-      <c r="C55" s="81"/>
-      <c r="D55" s="82"/>
+      <c r="B55" s="71"/>
+      <c r="C55" s="71"/>
+      <c r="D55" s="72"/>
     </row>
     <row r="56" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
@@ -2706,19 +2709,19 @@
       <c r="A59" s="21" t="s">
         <v>148</v>
       </c>
-      <c r="B59" s="61" t="s">
+      <c r="B59" s="73" t="s">
         <v>147</v>
       </c>
-      <c r="C59" s="62"/>
-      <c r="D59" s="63"/>
+      <c r="C59" s="74"/>
+      <c r="D59" s="75"/>
     </row>
     <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="80" t="s">
+      <c r="A60" s="70" t="s">
         <v>174</v>
       </c>
-      <c r="B60" s="81"/>
-      <c r="C60" s="81"/>
-      <c r="D60" s="82"/>
+      <c r="B60" s="71"/>
+      <c r="C60" s="71"/>
+      <c r="D60" s="72"/>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
@@ -2749,38 +2752,38 @@
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="102"/>
-      <c r="B63" s="102"/>
-      <c r="C63" s="102"/>
-      <c r="D63" s="102"/>
+      <c r="A63" s="92"/>
+      <c r="B63" s="92"/>
+      <c r="C63" s="92"/>
+      <c r="D63" s="92"/>
     </row>
     <row r="64" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="90" t="s">
+      <c r="A64" s="80" t="s">
         <v>7</v>
       </c>
-      <c r="B64" s="91"/>
-      <c r="C64" s="91"/>
-      <c r="D64" s="92"/>
+      <c r="B64" s="81"/>
+      <c r="C64" s="81"/>
+      <c r="D64" s="82"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B65" s="71" t="s">
+      <c r="B65" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="C65" s="72"/>
+      <c r="C65" s="99"/>
       <c r="D65" s="42"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B66" s="99" t="s">
+      <c r="B66" s="89" t="s">
         <v>53</v>
       </c>
-      <c r="C66" s="100"/>
-      <c r="D66" s="101"/>
+      <c r="C66" s="90"/>
+      <c r="D66" s="91"/>
     </row>
     <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="45" t="s">
@@ -2794,172 +2797,172 @@
     </row>
     <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="93" t="s">
+      <c r="A69" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="B69" s="94"/>
-      <c r="C69" s="94"/>
-      <c r="D69" s="95"/>
+      <c r="B69" s="84"/>
+      <c r="C69" s="84"/>
+      <c r="D69" s="85"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="96" t="s">
+      <c r="B70" s="86" t="s">
         <v>188</v>
       </c>
-      <c r="C70" s="97"/>
-      <c r="D70" s="98"/>
+      <c r="C70" s="87"/>
+      <c r="D70" s="88"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B71" s="58" t="s">
+      <c r="B71" s="61" t="s">
         <v>189</v>
       </c>
-      <c r="C71" s="59"/>
-      <c r="D71" s="60"/>
+      <c r="C71" s="62"/>
+      <c r="D71" s="63"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B72" s="58" t="s">
+      <c r="B72" s="61" t="s">
         <v>190</v>
       </c>
-      <c r="C72" s="59"/>
-      <c r="D72" s="60"/>
+      <c r="C72" s="62"/>
+      <c r="D72" s="63"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B73" s="58" t="s">
+      <c r="B73" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="C73" s="59"/>
-      <c r="D73" s="60"/>
+      <c r="C73" s="62"/>
+      <c r="D73" s="63"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B74" s="58" t="s">
+      <c r="B74" s="61" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="59"/>
-      <c r="D74" s="60"/>
+      <c r="C74" s="62"/>
+      <c r="D74" s="63"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B75" s="58" t="s">
+      <c r="B75" s="61" t="s">
         <v>70</v>
       </c>
-      <c r="C75" s="59"/>
-      <c r="D75" s="60"/>
+      <c r="C75" s="62"/>
+      <c r="D75" s="63"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B76" s="58" t="s">
+      <c r="B76" s="61" t="s">
         <v>191</v>
       </c>
-      <c r="C76" s="59"/>
-      <c r="D76" s="60"/>
+      <c r="C76" s="62"/>
+      <c r="D76" s="63"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B77" s="58" t="s">
+      <c r="B77" s="61" t="s">
         <v>71</v>
       </c>
-      <c r="C77" s="59"/>
-      <c r="D77" s="60"/>
+      <c r="C77" s="62"/>
+      <c r="D77" s="63"/>
     </row>
     <row r="78" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B78" s="58" t="s">
+      <c r="B78" s="61" t="s">
         <v>72</v>
       </c>
-      <c r="C78" s="59"/>
-      <c r="D78" s="60"/>
+      <c r="C78" s="62"/>
+      <c r="D78" s="63"/>
     </row>
     <row r="79" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B79" s="58" t="s">
+      <c r="B79" s="61" t="s">
         <v>159</v>
       </c>
-      <c r="C79" s="59"/>
-      <c r="D79" s="60"/>
+      <c r="C79" s="62"/>
+      <c r="D79" s="63"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="58" t="s">
+      <c r="B80" s="61" t="s">
         <v>160</v>
       </c>
-      <c r="C80" s="59"/>
-      <c r="D80" s="60"/>
+      <c r="C80" s="62"/>
+      <c r="D80" s="63"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="B81" s="58" t="s">
+      <c r="B81" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="C81" s="59"/>
-      <c r="D81" s="60"/>
+      <c r="C81" s="62"/>
+      <c r="D81" s="63"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="B82" s="58" t="s">
+      <c r="B82" s="61" t="s">
         <v>96</v>
       </c>
-      <c r="C82" s="59"/>
-      <c r="D82" s="60"/>
+      <c r="C82" s="62"/>
+      <c r="D82" s="63"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="B83" s="58" t="s">
+      <c r="B83" s="61" t="s">
         <v>133</v>
       </c>
-      <c r="C83" s="59"/>
-      <c r="D83" s="60"/>
+      <c r="C83" s="62"/>
+      <c r="D83" s="63"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="B84" s="58" t="s">
+      <c r="B84" s="61" t="s">
         <v>101</v>
       </c>
-      <c r="C84" s="59"/>
-      <c r="D84" s="60"/>
+      <c r="C84" s="62"/>
+      <c r="D84" s="63"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="B85" s="58" t="s">
+      <c r="B85" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="C85" s="59"/>
-      <c r="D85" s="60"/>
+      <c r="C85" s="62"/>
+      <c r="D85" s="63"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="49" t="s">
@@ -2985,59 +2988,76 @@
       <c r="A88" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="B88" s="58" t="s">
+      <c r="B88" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="C88" s="59"/>
-      <c r="D88" s="60"/>
+      <c r="C88" s="62"/>
+      <c r="D88" s="63"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="B89" s="58" t="s">
+      <c r="B89" s="61" t="s">
         <v>126</v>
       </c>
-      <c r="C89" s="59"/>
-      <c r="D89" s="60"/>
+      <c r="C89" s="62"/>
+      <c r="D89" s="63"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="B90" s="58" t="s">
+      <c r="B90" s="61" t="s">
         <v>124</v>
       </c>
-      <c r="C90" s="59"/>
-      <c r="D90" s="60"/>
+      <c r="C90" s="62"/>
+      <c r="D90" s="63"/>
     </row>
     <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="51" t="s">
         <v>158</v>
       </c>
-      <c r="B91" s="107" t="s">
+      <c r="B91" s="58" t="s">
         <v>167</v>
       </c>
-      <c r="C91" s="108"/>
-      <c r="D91" s="109"/>
+      <c r="C91" s="59"/>
+      <c r="D91" s="60"/>
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B85:D85"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B84:D84"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="D34:D35"/>
     <mergeCell ref="A60:D60"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="B72:D72"/>
@@ -3054,38 +3074,21 @@
     <mergeCell ref="A4:A11"/>
     <mergeCell ref="B4:B11"/>
     <mergeCell ref="D4:D11"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B84:D84"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B85:D85"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B90:D90"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
added TC5 and NavigationTree
</commit_message>
<xml_diff>
--- a/doc/TA.Final.TestCases.DoroshenkoDenis.xlsx
+++ b/doc/TA.Final.TestCases.DoroshenkoDenis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\NetcrackerLearningCenter\finalPractice\cucumber-selenium\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789B222E-1B36-455D-B6FB-E12A1A37EDCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{991DD6CF-2BD8-4769-84FA-5A9D22EF224E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-8010" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -312,12 +312,6 @@
     <t>TC_5.6</t>
   </si>
   <si>
-    <t>Name: "test_city_name"; Population: 999999</t>
-  </si>
-  <si>
-    <t>Name: "country" +  random alphanumeric  string(length = 6); Language: ru</t>
-  </si>
-  <si>
     <t>test data5</t>
   </si>
   <si>
@@ -669,6 +663,12 @@
   </si>
   <si>
     <t>2.  Point the mouse at Infrastructure Orders and click</t>
+  </si>
+  <si>
+    <t>Name: "test_Country"; Language: ru</t>
+  </si>
+  <si>
+    <t>Name: "test_City"; Population: 999999</t>
   </si>
 </sst>
 </file>
@@ -1381,7 +1381,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1550,6 +1550,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1631,6 +1634,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1699,12 +1708,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2050,8 +2053,8 @@
   </sheetPr>
   <dimension ref="A1:F91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:B40"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2082,12 +2085,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="86"/>
-      <c r="C2" s="86"/>
-      <c r="D2" s="87"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="90"/>
       <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
@@ -2096,82 +2099,82 @@
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="101" t="s">
+      <c r="B3" s="104" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="101"/>
-      <c r="D3" s="102"/>
+      <c r="C3" s="104"/>
+      <c r="D3" s="105"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="103" t="s">
+      <c r="A4" s="106" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="80" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="104" t="s">
+      <c r="D4" s="107" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="103"/>
-      <c r="B5" s="79"/>
+      <c r="A5" s="106"/>
+      <c r="B5" s="80"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="104"/>
+      <c r="D5" s="107"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="103"/>
-      <c r="B6" s="79"/>
+      <c r="A6" s="106"/>
+      <c r="B6" s="80"/>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="104"/>
+      <c r="D6" s="107"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="103"/>
-      <c r="B7" s="79"/>
+      <c r="A7" s="106"/>
+      <c r="B7" s="80"/>
       <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="104"/>
+      <c r="D7" s="107"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="103"/>
-      <c r="B8" s="79"/>
+      <c r="A8" s="106"/>
+      <c r="B8" s="80"/>
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="104"/>
+      <c r="D8" s="107"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="103"/>
-      <c r="B9" s="79"/>
+      <c r="A9" s="106"/>
+      <c r="B9" s="80"/>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="104"/>
+      <c r="D9" s="107"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="103"/>
-      <c r="B10" s="79"/>
+      <c r="A10" s="106"/>
+      <c r="B10" s="80"/>
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="104"/>
+      <c r="D10" s="107"/>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="103"/>
-      <c r="B11" s="79"/>
+      <c r="A11" s="106"/>
+      <c r="B11" s="80"/>
       <c r="C11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="104"/>
+      <c r="D11" s="107"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="52" t="s">
@@ -2205,81 +2208,81 @@
       <c r="A14" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="61" t="s">
+      <c r="B14" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="62"/>
-      <c r="D14" s="63"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="64"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="73" t="s">
+      <c r="A15" s="74" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="76" t="s">
-        <v>169</v>
+      <c r="B15" s="77" t="s">
+        <v>167</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="65" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="74"/>
-      <c r="B16" s="77"/>
+      <c r="A16" s="75"/>
+      <c r="B16" s="78"/>
       <c r="C16" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D16" s="65"/>
+        <v>168</v>
+      </c>
+      <c r="D16" s="66"/>
     </row>
     <row r="17" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="75"/>
-      <c r="B17" s="78"/>
+      <c r="A17" s="76"/>
+      <c r="B17" s="79"/>
       <c r="C17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="66"/>
+      <c r="D17" s="67"/>
     </row>
     <row r="18" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="61" t="s">
+      <c r="B18" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="62"/>
-      <c r="D18" s="63"/>
+      <c r="C18" s="63"/>
+      <c r="D18" s="64"/>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="67" t="s">
+      <c r="A19" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="68"/>
-      <c r="C19" s="68"/>
-      <c r="D19" s="69"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="70"/>
     </row>
     <row r="20" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="70" t="s">
+      <c r="A20" s="71" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="80" t="s">
         <v>80</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="64" t="s">
+      <c r="D20" s="65" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="70"/>
-      <c r="B21" s="79"/>
+      <c r="A21" s="71"/>
+      <c r="B21" s="80"/>
       <c r="C21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="65"/>
+      <c r="D21" s="66"/>
     </row>
     <row r="22" spans="1:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="54" t="s">
@@ -2291,47 +2294,47 @@
       <c r="C22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="66"/>
+      <c r="D22" s="67"/>
     </row>
     <row r="23" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="61" t="s">
+      <c r="B23" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="62"/>
-      <c r="D23" s="63"/>
+      <c r="C23" s="63"/>
+      <c r="D23" s="64"/>
     </row>
     <row r="24" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="67" t="s">
+      <c r="A24" s="68" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="68"/>
-      <c r="C24" s="68"/>
-      <c r="D24" s="69"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="70"/>
     </row>
     <row r="25" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="70" t="s">
+      <c r="A25" s="71" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="79" t="s">
+      <c r="B25" s="80" t="s">
         <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="D25" s="64" t="s">
+        <v>185</v>
+      </c>
+      <c r="D25" s="65" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="70"/>
-      <c r="B26" s="79"/>
+      <c r="A26" s="71"/>
+      <c r="B26" s="80"/>
       <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="65"/>
+      <c r="D26" s="66"/>
     </row>
     <row r="27" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="56" t="s">
@@ -2343,7 +2346,7 @@
       <c r="C27" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="65"/>
+      <c r="D27" s="66"/>
     </row>
     <row r="28" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="55" t="s">
@@ -2355,7 +2358,7 @@
       <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="65"/>
+      <c r="D28" s="66"/>
     </row>
     <row r="29" spans="1:4" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="57" t="s">
@@ -2367,179 +2370,179 @@
       <c r="C29" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="66"/>
+      <c r="D29" s="67"/>
     </row>
     <row r="30" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="61" t="s">
-        <v>135</v>
-      </c>
-      <c r="C30" s="62"/>
-      <c r="D30" s="63"/>
+      <c r="B30" s="62" t="s">
+        <v>133</v>
+      </c>
+      <c r="C30" s="63"/>
+      <c r="D30" s="64"/>
     </row>
     <row r="31" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="80" t="s">
-        <v>172</v>
-      </c>
-      <c r="B31" s="81"/>
-      <c r="C31" s="81"/>
-      <c r="D31" s="82"/>
+      <c r="A31" s="81" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" s="82"/>
+      <c r="C31" s="82"/>
+      <c r="D31" s="83"/>
     </row>
     <row r="32" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="108" t="s">
+      <c r="A32" s="86" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="76" t="s">
+      <c r="B32" s="77" t="s">
         <v>84</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="64" t="s">
+      <c r="D32" s="65" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="109"/>
-      <c r="B33" s="84"/>
+      <c r="A33" s="87"/>
+      <c r="B33" s="85"/>
       <c r="C33" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="83"/>
+      <c r="D33" s="84"/>
     </row>
     <row r="34" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="108" t="s">
+      <c r="A34" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="76" t="s">
+      <c r="B34" s="77" t="s">
         <v>85</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="64" t="s">
+      <c r="D34" s="65" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="109"/>
-      <c r="B35" s="84"/>
+      <c r="A35" s="87"/>
+      <c r="B35" s="85"/>
       <c r="C35" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D35" s="83"/>
+        <v>190</v>
+      </c>
+      <c r="D35" s="84"/>
     </row>
     <row r="36" spans="1:4" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="58" t="s">
         <v>93</v>
       </c>
       <c r="B36" s="29" t="s">
         <v>94</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D36" s="23" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="B37" s="76" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="B37" s="77" t="s">
+        <v>115</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>121</v>
-      </c>
-      <c r="D37" s="64" t="s">
-        <v>110</v>
+        <v>119</v>
+      </c>
+      <c r="D37" s="65" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="26" t="s">
-        <v>115</v>
-      </c>
-      <c r="B38" s="77"/>
+        <v>113</v>
+      </c>
+      <c r="B38" s="78"/>
       <c r="C38" s="27" t="s">
-        <v>122</v>
-      </c>
-      <c r="D38" s="65"/>
+        <v>120</v>
+      </c>
+      <c r="D38" s="66"/>
     </row>
     <row r="39" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="26" t="s">
-        <v>116</v>
-      </c>
-      <c r="B39" s="77"/>
+        <v>114</v>
+      </c>
+      <c r="B39" s="78"/>
       <c r="C39" s="27" t="s">
-        <v>120</v>
-      </c>
-      <c r="D39" s="65"/>
+        <v>118</v>
+      </c>
+      <c r="D39" s="66"/>
     </row>
     <row r="40" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="B40" s="84"/>
+        <v>116</v>
+      </c>
+      <c r="B40" s="85"/>
       <c r="C40" s="27" t="s">
-        <v>123</v>
-      </c>
-      <c r="D40" s="83"/>
+        <v>121</v>
+      </c>
+      <c r="D40" s="84"/>
     </row>
     <row r="41" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="80" t="s">
-        <v>127</v>
-      </c>
-      <c r="B41" s="81"/>
-      <c r="C41" s="81"/>
-      <c r="D41" s="82"/>
+      <c r="A41" s="81" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="82"/>
+      <c r="C41" s="82"/>
+      <c r="D41" s="83"/>
     </row>
     <row r="42" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="B42" s="76" t="s">
-        <v>165</v>
+        <v>126</v>
+      </c>
+      <c r="B42" s="77" t="s">
+        <v>163</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>129</v>
-      </c>
-      <c r="D42" s="64" t="s">
-        <v>103</v>
+        <v>127</v>
+      </c>
+      <c r="D42" s="65" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
-        <v>164</v>
-      </c>
-      <c r="B43" s="77"/>
+        <v>162</v>
+      </c>
+      <c r="B43" s="78"/>
       <c r="C43" s="27" t="s">
-        <v>130</v>
-      </c>
-      <c r="D43" s="65"/>
+        <v>128</v>
+      </c>
+      <c r="D43" s="66"/>
     </row>
     <row r="44" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="26" t="s">
-        <v>163</v>
-      </c>
-      <c r="B44" s="84"/>
+        <v>161</v>
+      </c>
+      <c r="B44" s="85"/>
       <c r="C44" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="D44" s="83"/>
+        <v>129</v>
+      </c>
+      <c r="D44" s="84"/>
     </row>
     <row r="45" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="26" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="29" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D45" s="23" t="s">
         <v>86</v>
@@ -2547,13 +2550,13 @@
     </row>
     <row r="46" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="B46" s="37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C46" s="38" t="s">
         <v>105</v>
-      </c>
-      <c r="B46" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="C46" s="38" t="s">
-        <v>107</v>
       </c>
       <c r="D46" s="39" t="s">
         <v>87</v>
@@ -2561,85 +2564,85 @@
     </row>
     <row r="47" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="21" t="s">
+        <v>132</v>
+      </c>
+      <c r="B47" s="62" t="s">
         <v>134</v>
       </c>
-      <c r="B47" s="61" t="s">
-        <v>136</v>
-      </c>
-      <c r="C47" s="62"/>
-      <c r="D47" s="63"/>
+      <c r="C47" s="63"/>
+      <c r="D47" s="64"/>
     </row>
     <row r="48" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="80" t="s">
-        <v>173</v>
-      </c>
-      <c r="B48" s="81"/>
-      <c r="C48" s="81"/>
-      <c r="D48" s="82"/>
+      <c r="A48" s="81" t="s">
+        <v>171</v>
+      </c>
+      <c r="B48" s="82"/>
+      <c r="C48" s="82"/>
+      <c r="D48" s="83"/>
     </row>
     <row r="49" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C49" s="28" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D49" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B50" s="31" t="s">
+        <v>151</v>
+      </c>
+      <c r="C50" s="28" t="s">
         <v>153</v>
       </c>
-      <c r="C50" s="28" t="s">
-        <v>155</v>
-      </c>
       <c r="D50" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C51" s="28" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D51" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B52" s="31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C52" s="28" t="s">
         <v>166</v>
-      </c>
-      <c r="C52" s="28" t="s">
-        <v>168</v>
       </c>
       <c r="D52" s="14"/>
     </row>
     <row r="53" spans="1:4" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="18" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B53" s="31" t="s">
+        <v>167</v>
+      </c>
+      <c r="C53" s="28" t="s">
         <v>169</v>
-      </c>
-      <c r="C53" s="28" t="s">
-        <v>171</v>
       </c>
       <c r="D53" s="14" t="s">
         <v>48</v>
@@ -2647,91 +2650,91 @@
     </row>
     <row r="54" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="B54" s="61" t="s">
-        <v>142</v>
-      </c>
-      <c r="C54" s="62"/>
-      <c r="D54" s="63"/>
+        <v>141</v>
+      </c>
+      <c r="B54" s="62" t="s">
+        <v>140</v>
+      </c>
+      <c r="C54" s="63"/>
+      <c r="D54" s="64"/>
     </row>
     <row r="55" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="80" t="s">
-        <v>175</v>
-      </c>
-      <c r="B55" s="81"/>
-      <c r="C55" s="81"/>
-      <c r="D55" s="82"/>
+      <c r="A55" s="81" t="s">
+        <v>173</v>
+      </c>
+      <c r="B55" s="82"/>
+      <c r="C55" s="82"/>
+      <c r="D55" s="83"/>
     </row>
     <row r="56" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B56" s="31" t="s">
+        <v>175</v>
+      </c>
+      <c r="C56" s="28" t="s">
         <v>177</v>
       </c>
-      <c r="C56" s="28" t="s">
-        <v>179</v>
-      </c>
       <c r="D56" s="14" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B57" s="31" t="s">
+        <v>176</v>
+      </c>
+      <c r="C57" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="C57" s="28" t="s">
+      <c r="D57" s="14" t="s">
         <v>180</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="18" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C58" s="28" t="s">
+        <v>179</v>
+      </c>
+      <c r="D58" s="14" t="s">
         <v>181</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
-        <v>148</v>
-      </c>
-      <c r="B59" s="61" t="s">
-        <v>147</v>
-      </c>
-      <c r="C59" s="62"/>
-      <c r="D59" s="63"/>
+        <v>146</v>
+      </c>
+      <c r="B59" s="62" t="s">
+        <v>145</v>
+      </c>
+      <c r="C59" s="63"/>
+      <c r="D59" s="64"/>
     </row>
     <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="80" t="s">
-        <v>174</v>
-      </c>
-      <c r="B60" s="81"/>
-      <c r="C60" s="81"/>
-      <c r="D60" s="82"/>
+      <c r="A60" s="81" t="s">
+        <v>172</v>
+      </c>
+      <c r="B60" s="82"/>
+      <c r="C60" s="82"/>
+      <c r="D60" s="83"/>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B61" s="43" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C61" s="28" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D61" s="14" t="s">
         <v>29</v>
@@ -2739,51 +2742,51 @@
     </row>
     <row r="62" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B62" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="C62" s="38" t="s">
         <v>184</v>
-      </c>
-      <c r="C62" s="38" t="s">
-        <v>186</v>
       </c>
       <c r="D62" s="40" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="100"/>
-      <c r="B63" s="100"/>
-      <c r="C63" s="100"/>
-      <c r="D63" s="100"/>
+      <c r="A63" s="103"/>
+      <c r="B63" s="103"/>
+      <c r="C63" s="103"/>
+      <c r="D63" s="103"/>
     </row>
     <row r="64" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="88" t="s">
+      <c r="A64" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="B64" s="89"/>
-      <c r="C64" s="89"/>
-      <c r="D64" s="90"/>
+      <c r="B64" s="92"/>
+      <c r="C64" s="92"/>
+      <c r="D64" s="93"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B65" s="71" t="s">
+      <c r="B65" s="72" t="s">
         <v>49</v>
       </c>
-      <c r="C65" s="72"/>
+      <c r="C65" s="73"/>
       <c r="D65" s="42"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B66" s="97" t="s">
+      <c r="B66" s="100" t="s">
         <v>53</v>
       </c>
-      <c r="C66" s="98"/>
-      <c r="D66" s="99"/>
+      <c r="C66" s="101"/>
+      <c r="D66" s="102"/>
     </row>
     <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="45" t="s">
@@ -2797,232 +2800,232 @@
     </row>
     <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="91" t="s">
+      <c r="A69" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="B69" s="92"/>
-      <c r="C69" s="92"/>
-      <c r="D69" s="93"/>
+      <c r="B69" s="95"/>
+      <c r="C69" s="95"/>
+      <c r="D69" s="96"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="94" t="s">
-        <v>188</v>
-      </c>
-      <c r="C70" s="95"/>
-      <c r="D70" s="96"/>
+      <c r="B70" s="97" t="s">
+        <v>186</v>
+      </c>
+      <c r="C70" s="98"/>
+      <c r="D70" s="99"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="B71" s="58" t="s">
-        <v>189</v>
-      </c>
-      <c r="C71" s="59"/>
-      <c r="D71" s="60"/>
+      <c r="B71" s="59" t="s">
+        <v>187</v>
+      </c>
+      <c r="C71" s="60"/>
+      <c r="D71" s="61"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="B72" s="58" t="s">
-        <v>190</v>
-      </c>
-      <c r="C72" s="59"/>
-      <c r="D72" s="60"/>
+      <c r="B72" s="59" t="s">
+        <v>188</v>
+      </c>
+      <c r="C72" s="60"/>
+      <c r="D72" s="61"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="B73" s="58" t="s">
+      <c r="B73" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C73" s="59"/>
-      <c r="D73" s="60"/>
+      <c r="C73" s="60"/>
+      <c r="D73" s="61"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="B74" s="58" t="s">
+      <c r="B74" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="59"/>
-      <c r="D74" s="60"/>
+      <c r="C74" s="60"/>
+      <c r="D74" s="61"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="B75" s="58" t="s">
+      <c r="B75" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="C75" s="59"/>
-      <c r="D75" s="60"/>
+      <c r="C75" s="60"/>
+      <c r="D75" s="61"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="B76" s="58" t="s">
-        <v>191</v>
-      </c>
-      <c r="C76" s="59"/>
-      <c r="D76" s="60"/>
+      <c r="B76" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="C76" s="60"/>
+      <c r="D76" s="61"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="B77" s="58" t="s">
+      <c r="B77" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="C77" s="59"/>
-      <c r="D77" s="60"/>
+      <c r="C77" s="60"/>
+      <c r="D77" s="61"/>
     </row>
     <row r="78" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="B78" s="58" t="s">
+      <c r="B78" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="C78" s="59"/>
-      <c r="D78" s="60"/>
+      <c r="C78" s="60"/>
+      <c r="D78" s="61"/>
     </row>
     <row r="79" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="B79" s="58" t="s">
-        <v>159</v>
-      </c>
-      <c r="C79" s="59"/>
-      <c r="D79" s="60"/>
+      <c r="B79" s="59" t="s">
+        <v>157</v>
+      </c>
+      <c r="C79" s="60"/>
+      <c r="D79" s="61"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="58" t="s">
-        <v>160</v>
-      </c>
-      <c r="C80" s="59"/>
-      <c r="D80" s="60"/>
+      <c r="B80" s="59" t="s">
+        <v>158</v>
+      </c>
+      <c r="C80" s="60"/>
+      <c r="D80" s="61"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="B81" s="58" t="s">
-        <v>97</v>
-      </c>
-      <c r="C81" s="59"/>
-      <c r="D81" s="60"/>
+      <c r="B81" s="59" t="s">
+        <v>191</v>
+      </c>
+      <c r="C81" s="60"/>
+      <c r="D81" s="61"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="B82" s="58" t="s">
-        <v>96</v>
-      </c>
-      <c r="C82" s="59"/>
-      <c r="D82" s="60"/>
+      <c r="B82" s="59" t="s">
+        <v>192</v>
+      </c>
+      <c r="C82" s="60"/>
+      <c r="D82" s="61"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="B83" s="58" t="s">
-        <v>133</v>
-      </c>
-      <c r="C83" s="59"/>
-      <c r="D83" s="60"/>
+      <c r="B83" s="59" t="s">
+        <v>131</v>
+      </c>
+      <c r="C83" s="60"/>
+      <c r="D83" s="61"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="B84" s="58" t="s">
-        <v>101</v>
-      </c>
-      <c r="C84" s="59"/>
-      <c r="D84" s="60"/>
+      <c r="B84" s="59" t="s">
+        <v>99</v>
+      </c>
+      <c r="C84" s="60"/>
+      <c r="D84" s="61"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="B85" s="58" t="s">
-        <v>111</v>
-      </c>
-      <c r="C85" s="59"/>
-      <c r="D85" s="60"/>
+        <v>96</v>
+      </c>
+      <c r="B85" s="59" t="s">
+        <v>109</v>
+      </c>
+      <c r="C85" s="60"/>
+      <c r="D85" s="61"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="49" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B86" s="35" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C86" s="36"/>
       <c r="D86" s="50"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="49" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B87" s="15" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C87" s="16"/>
       <c r="D87" s="50"/>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="B88" s="58" t="s">
-        <v>108</v>
-      </c>
-      <c r="C88" s="59"/>
-      <c r="D88" s="60"/>
+        <v>107</v>
+      </c>
+      <c r="B88" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="C88" s="60"/>
+      <c r="D88" s="61"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="49" t="s">
-        <v>112</v>
-      </c>
-      <c r="B89" s="58" t="s">
-        <v>126</v>
-      </c>
-      <c r="C89" s="59"/>
-      <c r="D89" s="60"/>
+        <v>110</v>
+      </c>
+      <c r="B89" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="C89" s="60"/>
+      <c r="D89" s="61"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="49" t="s">
-        <v>119</v>
-      </c>
-      <c r="B90" s="58" t="s">
-        <v>124</v>
-      </c>
-      <c r="C90" s="59"/>
-      <c r="D90" s="60"/>
+        <v>117</v>
+      </c>
+      <c r="B90" s="59" t="s">
+        <v>122</v>
+      </c>
+      <c r="C90" s="60"/>
+      <c r="D90" s="61"/>
     </row>
     <row r="91" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="51" t="s">
-        <v>158</v>
-      </c>
-      <c r="B91" s="105" t="s">
-        <v>167</v>
-      </c>
-      <c r="C91" s="106"/>
-      <c r="D91" s="107"/>
+        <v>156</v>
+      </c>
+      <c r="B91" s="108" t="s">
+        <v>165</v>
+      </c>
+      <c r="C91" s="109"/>
+      <c r="D91" s="110"/>
     </row>
   </sheetData>
   <mergeCells count="63">

</xml_diff>

<commit_message>
added all TC 5
</commit_message>
<xml_diff>
--- a/doc/TA.Final.TestCases.DoroshenkoDenis.xlsx
+++ b/doc/TA.Final.TestCases.DoroshenkoDenis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\NetcrackerLearningCenter\finalPractice\cucumber-selenium\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9849F3B0-9C15-4EF8-AD38-15D0DB2306B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A23E85-5D86-4774-8101-CD8D665CAB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-8010" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -631,9 +631,6 @@
     <t>Number: "1"; Square: "1000"</t>
   </si>
   <si>
-    <t>Name: "Torre InterPlaza"; Street Name: "Boulevard Juan Pablo"; Number: "1"; Square:10000; Is connected: Lit</t>
-  </si>
-  <si>
     <t>test data12</t>
   </si>
   <si>
@@ -675,6 +672,9 @@
   </si>
   <si>
     <t>The search results should contain object-link with test data6</t>
+  </si>
+  <si>
+    <t>Name: "Torre InterPlaza"; Street Name: "Boulevard Juan Pablo"; Is connected: Lit</t>
   </si>
 </sst>
 </file>
@@ -725,7 +725,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -774,6 +774,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="48">
     <border>
@@ -1387,7 +1393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="114">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1448,9 +1454,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1460,9 +1463,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1568,6 +1568,162 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1576,153 +1732,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="44" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="35" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="8" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2068,8 +2077,8 @@
   </sheetPr>
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37:B40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2086,7 +2095,7 @@
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="28" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="12" t="s">
@@ -2100,12 +2109,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="80" t="s">
+      <c r="A2" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="81"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="82"/>
+      <c r="B2" s="93"/>
+      <c r="C2" s="93"/>
+      <c r="D2" s="94"/>
       <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
@@ -2114,88 +2123,88 @@
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B3" s="108" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="99"/>
+      <c r="C3" s="108"/>
+      <c r="D3" s="109"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="100" t="s">
+      <c r="A4" s="110" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="83" t="s">
+      <c r="B4" s="84" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="101" t="s">
+      <c r="D4" s="111" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="100"/>
-      <c r="B5" s="83"/>
+      <c r="A5" s="110"/>
+      <c r="B5" s="84"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="101"/>
+      <c r="D5" s="111"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="100"/>
-      <c r="B6" s="83"/>
+      <c r="A6" s="110"/>
+      <c r="B6" s="84"/>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="101"/>
+      <c r="D6" s="111"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="100"/>
-      <c r="B7" s="83"/>
+      <c r="A7" s="110"/>
+      <c r="B7" s="84"/>
       <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="101"/>
+      <c r="D7" s="111"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="100"/>
-      <c r="B8" s="83"/>
+      <c r="A8" s="110"/>
+      <c r="B8" s="84"/>
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="101"/>
+      <c r="D8" s="111"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="100"/>
-      <c r="B9" s="83"/>
+      <c r="A9" s="110"/>
+      <c r="B9" s="84"/>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="101"/>
+      <c r="D9" s="111"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="100"/>
-      <c r="B10" s="83"/>
+      <c r="A10" s="110"/>
+      <c r="B10" s="84"/>
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="101"/>
+      <c r="D10" s="111"/>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="100"/>
-      <c r="B11" s="83"/>
+      <c r="A11" s="110"/>
+      <c r="B11" s="84"/>
       <c r="C11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="101"/>
+      <c r="D11" s="111"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -2206,10 +2215,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="52" t="s">
+      <c r="A13" s="50" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="30" t="s">
         <v>28</v>
       </c>
       <c r="C13" s="10" t="s">
@@ -2223,357 +2232,357 @@
       <c r="A14" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="77" t="s">
+      <c r="B14" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="78"/>
-      <c r="D14" s="79"/>
+      <c r="C14" s="67"/>
+      <c r="D14" s="68"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="104" t="s">
+      <c r="A15" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="81" t="s">
         <v>158</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="71" t="s">
+      <c r="D15" s="69" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="105"/>
-      <c r="B16" s="69"/>
+      <c r="A16" s="79"/>
+      <c r="B16" s="82"/>
       <c r="C16" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="D16" s="72"/>
+      <c r="D16" s="70"/>
     </row>
     <row r="17" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="106"/>
-      <c r="B17" s="107"/>
+      <c r="A17" s="80"/>
+      <c r="B17" s="83"/>
       <c r="C17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="111"/>
+      <c r="D17" s="71"/>
     </row>
     <row r="18" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="77" t="s">
+      <c r="B18" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="78"/>
-      <c r="D18" s="79"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="68"/>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="108" t="s">
+      <c r="A19" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="109"/>
-      <c r="C19" s="109"/>
-      <c r="D19" s="110"/>
+      <c r="B19" s="73"/>
+      <c r="C19" s="73"/>
+      <c r="D19" s="74"/>
     </row>
     <row r="20" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="97" t="s">
+      <c r="A20" s="75" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="83" t="s">
+      <c r="B20" s="84" t="s">
         <v>80</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="71" t="s">
+      <c r="D20" s="69" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="97"/>
-      <c r="B21" s="83"/>
+      <c r="A21" s="75"/>
+      <c r="B21" s="84"/>
       <c r="C21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="72"/>
+      <c r="D21" s="70"/>
     </row>
     <row r="22" spans="1:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="51" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="33" t="s">
+      <c r="B22" s="31" t="s">
         <v>79</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="111"/>
+      <c r="D22" s="71"/>
     </row>
     <row r="23" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="77" t="s">
+      <c r="B23" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="78"/>
-      <c r="D23" s="79"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="68"/>
     </row>
     <row r="24" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="108" t="s">
+      <c r="A24" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="109"/>
-      <c r="C24" s="109"/>
-      <c r="D24" s="110"/>
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="74"/>
     </row>
     <row r="25" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="97" t="s">
+      <c r="A25" s="75" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="83" t="s">
+      <c r="B25" s="84" t="s">
         <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="D25" s="71" t="s">
+      <c r="D25" s="69" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="97"/>
-      <c r="B26" s="83"/>
+      <c r="A26" s="75"/>
+      <c r="B26" s="84"/>
       <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="72"/>
+      <c r="D26" s="70"/>
     </row>
     <row r="27" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="55" t="s">
+      <c r="A27" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="72"/>
+      <c r="D27" s="70"/>
     </row>
     <row r="28" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="B28" s="31" t="s">
+      <c r="B28" s="29" t="s">
         <v>77</v>
       </c>
       <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="72"/>
+      <c r="D28" s="70"/>
     </row>
     <row r="29" spans="1:4" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="54" t="s">
         <v>64</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="25" t="s">
+      <c r="C29" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="111"/>
+      <c r="D29" s="71"/>
     </row>
     <row r="30" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="77" t="s">
+      <c r="B30" s="66" t="s">
         <v>124</v>
       </c>
-      <c r="C30" s="78"/>
-      <c r="D30" s="79"/>
+      <c r="C30" s="67"/>
+      <c r="D30" s="68"/>
     </row>
     <row r="31" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="85" t="s">
         <v>161</v>
       </c>
-      <c r="B31" s="75"/>
-      <c r="C31" s="75"/>
-      <c r="D31" s="76"/>
+      <c r="B31" s="86"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="87"/>
     </row>
     <row r="32" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="112" t="s">
+      <c r="A32" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="81" t="s">
         <v>84</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="71" t="s">
+      <c r="D32" s="69" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="113"/>
-      <c r="B33" s="70"/>
+      <c r="A33" s="91"/>
+      <c r="B33" s="89"/>
       <c r="C33" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="73"/>
+      <c r="D33" s="88"/>
     </row>
     <row r="34" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="112" t="s">
+      <c r="A34" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="68" t="s">
+      <c r="B34" s="81" t="s">
         <v>85</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="71" t="s">
+      <c r="D34" s="69" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="113"/>
-      <c r="B35" s="70"/>
+      <c r="A35" s="91"/>
+      <c r="B35" s="89"/>
       <c r="C35" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="D35" s="73"/>
+      <c r="D35" s="88"/>
     </row>
     <row r="36" spans="1:4" ht="162" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="B36" s="29" t="s">
+      <c r="B36" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C36" s="27" t="s">
-        <v>187</v>
-      </c>
-      <c r="D36" s="23" t="s">
+      <c r="C36" s="25" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" s="22" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="61" t="s">
+      <c r="A37" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="B37" s="68" t="s">
+      <c r="B37" s="81" t="s">
         <v>113</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="D37" s="69" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="59" t="s">
+        <v>111</v>
+      </c>
+      <c r="B38" s="82"/>
+      <c r="C38" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="D37" s="71" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="B38" s="69"/>
-      <c r="C38" s="27" t="s">
+      <c r="D38" s="70"/>
+    </row>
+    <row r="39" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="59" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="82"/>
+      <c r="C39" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="D38" s="72"/>
-    </row>
-    <row r="39" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="61" t="s">
-        <v>112</v>
-      </c>
-      <c r="B39" s="69"/>
-      <c r="C39" s="27" t="s">
+      <c r="D39" s="70"/>
+    </row>
+    <row r="40" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="59" t="s">
+        <v>114</v>
+      </c>
+      <c r="B40" s="89"/>
+      <c r="C40" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="D39" s="72"/>
-    </row>
-    <row r="40" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="61" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" s="70"/>
-      <c r="C40" s="27" t="s">
-        <v>192</v>
-      </c>
-      <c r="D40" s="73"/>
+      <c r="D40" s="88"/>
     </row>
     <row r="41" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="74" t="s">
+      <c r="A41" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="B41" s="75"/>
-      <c r="C41" s="75"/>
-      <c r="D41" s="76"/>
+      <c r="B41" s="86"/>
+      <c r="C41" s="86"/>
+      <c r="D41" s="87"/>
     </row>
     <row r="42" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="26" t="s">
+      <c r="A42" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="68" t="s">
+      <c r="B42" s="81" t="s">
         <v>154</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="71" t="s">
+      <c r="D42" s="69" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="26" t="s">
+      <c r="A43" s="60" t="s">
         <v>153</v>
       </c>
-      <c r="B43" s="69"/>
-      <c r="C43" s="27" t="s">
+      <c r="B43" s="82"/>
+      <c r="C43" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="72"/>
+      <c r="D43" s="70"/>
     </row>
     <row r="44" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="26" t="s">
+      <c r="A44" s="60" t="s">
         <v>152</v>
       </c>
-      <c r="B44" s="70"/>
-      <c r="C44" s="27" t="s">
+      <c r="B44" s="89"/>
+      <c r="C44" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="D44" s="73"/>
+      <c r="D44" s="88"/>
     </row>
     <row r="45" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="26" t="s">
+      <c r="A45" s="62" t="s">
         <v>95</v>
       </c>
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="C45" s="27" t="s">
+      <c r="C45" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="D45" s="23" t="s">
+      <c r="D45" s="22" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="22" t="s">
+      <c r="A46" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="B46" s="37" t="s">
+      <c r="B46" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="C46" s="38" t="s">
+      <c r="C46" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="D46" s="39" t="s">
+      <c r="D46" s="37" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2581,28 +2590,28 @@
       <c r="A47" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="B47" s="77" t="s">
+      <c r="B47" s="66" t="s">
         <v>125</v>
       </c>
-      <c r="C47" s="78"/>
-      <c r="D47" s="79"/>
+      <c r="C47" s="67"/>
+      <c r="D47" s="68"/>
     </row>
     <row r="48" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="74" t="s">
+      <c r="A48" s="85" t="s">
         <v>162</v>
       </c>
-      <c r="B48" s="75"/>
-      <c r="C48" s="75"/>
-      <c r="D48" s="76"/>
+      <c r="B48" s="86"/>
+      <c r="C48" s="86"/>
+      <c r="D48" s="87"/>
     </row>
     <row r="49" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="31" t="s">
+      <c r="B49" s="29" t="s">
         <v>140</v>
       </c>
-      <c r="C49" s="28" t="s">
+      <c r="C49" s="26" t="s">
         <v>143</v>
       </c>
       <c r="D49" s="14" t="s">
@@ -2613,10 +2622,10 @@
       <c r="A50" s="18" t="s">
         <v>127</v>
       </c>
-      <c r="B50" s="31" t="s">
+      <c r="B50" s="29" t="s">
         <v>142</v>
       </c>
-      <c r="C50" s="28" t="s">
+      <c r="C50" s="26" t="s">
         <v>144</v>
       </c>
       <c r="D50" s="14" t="s">
@@ -2627,10 +2636,10 @@
       <c r="A51" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="B51" s="31" t="s">
+      <c r="B51" s="29" t="s">
         <v>146</v>
       </c>
-      <c r="C51" s="28" t="s">
+      <c r="C51" s="26" t="s">
         <v>150</v>
       </c>
       <c r="D51" s="14" t="s">
@@ -2641,22 +2650,22 @@
       <c r="A52" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B52" s="31" t="s">
+      <c r="B52" s="29" t="s">
         <v>155</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C52" s="26" t="s">
         <v>157</v>
       </c>
       <c r="D52" s="14"/>
     </row>
     <row r="53" spans="1:4" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="61" t="s">
         <v>130</v>
       </c>
-      <c r="B53" s="31" t="s">
+      <c r="B53" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="C53" s="28" t="s">
+      <c r="C53" s="26" t="s">
         <v>160</v>
       </c>
       <c r="D53" s="14" t="s">
@@ -2667,28 +2676,28 @@
       <c r="A54" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="77" t="s">
+      <c r="B54" s="66" t="s">
         <v>131</v>
       </c>
-      <c r="C54" s="78"/>
-      <c r="D54" s="79"/>
+      <c r="C54" s="67"/>
+      <c r="D54" s="68"/>
     </row>
     <row r="55" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="74" t="s">
+      <c r="A55" s="85" t="s">
         <v>164</v>
       </c>
-      <c r="B55" s="75"/>
-      <c r="C55" s="75"/>
-      <c r="D55" s="76"/>
+      <c r="B55" s="86"/>
+      <c r="C55" s="86"/>
+      <c r="D55" s="87"/>
     </row>
     <row r="56" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
         <v>133</v>
       </c>
-      <c r="B56" s="31" t="s">
+      <c r="B56" s="29" t="s">
         <v>166</v>
       </c>
-      <c r="C56" s="28" t="s">
+      <c r="C56" s="26" t="s">
         <v>168</v>
       </c>
       <c r="D56" s="14" t="s">
@@ -2699,10 +2708,10 @@
       <c r="A57" s="18" t="s">
         <v>134</v>
       </c>
-      <c r="B57" s="31" t="s">
+      <c r="B57" s="29" t="s">
         <v>167</v>
       </c>
-      <c r="C57" s="28" t="s">
+      <c r="C57" s="26" t="s">
         <v>169</v>
       </c>
       <c r="D57" s="14" t="s">
@@ -2713,10 +2722,10 @@
       <c r="A58" s="18" t="s">
         <v>135</v>
       </c>
-      <c r="B58" s="31" t="s">
+      <c r="B58" s="29" t="s">
         <v>165</v>
       </c>
-      <c r="C58" s="28" t="s">
+      <c r="C58" s="26" t="s">
         <v>170</v>
       </c>
       <c r="D58" s="14" t="s">
@@ -2727,28 +2736,28 @@
       <c r="A59" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="B59" s="77" t="s">
+      <c r="B59" s="66" t="s">
         <v>136</v>
       </c>
-      <c r="C59" s="78"/>
-      <c r="D59" s="79"/>
+      <c r="C59" s="67"/>
+      <c r="D59" s="68"/>
     </row>
     <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="74" t="s">
+      <c r="A60" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="B60" s="75"/>
-      <c r="C60" s="75"/>
-      <c r="D60" s="76"/>
+      <c r="B60" s="86"/>
+      <c r="C60" s="86"/>
+      <c r="D60" s="87"/>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="B61" s="43" t="s">
+      <c r="B61" s="41" t="s">
         <v>174</v>
       </c>
-      <c r="C61" s="28" t="s">
+      <c r="C61" s="26" t="s">
         <v>175</v>
       </c>
       <c r="D61" s="14" t="s">
@@ -2759,301 +2768,348 @@
       <c r="A62" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="B62" s="44" t="s">
+      <c r="B62" s="42" t="s">
         <v>173</v>
       </c>
-      <c r="C62" s="38" t="s">
+      <c r="C62" s="36" t="s">
         <v>175</v>
       </c>
-      <c r="D62" s="40" t="s">
+      <c r="D62" s="38" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="96"/>
-      <c r="B63" s="96"/>
-      <c r="C63" s="96"/>
-      <c r="D63" s="96"/>
+      <c r="A63" s="107"/>
+      <c r="B63" s="107"/>
+      <c r="C63" s="107"/>
+      <c r="D63" s="107"/>
     </row>
     <row r="64" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="84" t="s">
+      <c r="A64" s="95" t="s">
         <v>7</v>
       </c>
-      <c r="B64" s="85"/>
-      <c r="C64" s="85"/>
-      <c r="D64" s="86"/>
+      <c r="B64" s="96"/>
+      <c r="C64" s="96"/>
+      <c r="D64" s="97"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="41" t="s">
+      <c r="A65" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B65" s="102" t="s">
+      <c r="B65" s="76" t="s">
         <v>49</v>
       </c>
-      <c r="C65" s="103"/>
-      <c r="D65" s="42"/>
+      <c r="C65" s="77"/>
+      <c r="D65" s="40"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="41" t="s">
+      <c r="A66" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B66" s="93" t="s">
+      <c r="B66" s="104" t="s">
         <v>53</v>
       </c>
-      <c r="C66" s="94"/>
-      <c r="D66" s="95"/>
+      <c r="C66" s="105"/>
+      <c r="D66" s="106"/>
     </row>
     <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="45" t="s">
+      <c r="A67" s="43" t="s">
         <v>58</v>
       </c>
-      <c r="B67" s="46" t="s">
+      <c r="B67" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="C67" s="47"/>
-      <c r="D67" s="48"/>
+      <c r="C67" s="45"/>
+      <c r="D67" s="46"/>
     </row>
     <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="87" t="s">
+      <c r="A69" s="98" t="s">
         <v>5</v>
       </c>
-      <c r="B69" s="88"/>
-      <c r="C69" s="88"/>
-      <c r="D69" s="89"/>
+      <c r="B69" s="99"/>
+      <c r="C69" s="99"/>
+      <c r="D69" s="100"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="49" t="s">
+      <c r="A70" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="90" t="s">
+      <c r="B70" s="101" t="s">
         <v>177</v>
       </c>
-      <c r="C70" s="91"/>
-      <c r="D70" s="92"/>
+      <c r="C70" s="102"/>
+      <c r="D70" s="103"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="49" t="s">
+      <c r="A71" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B71" s="65" t="s">
+      <c r="B71" s="63" t="s">
         <v>178</v>
       </c>
-      <c r="C71" s="66"/>
-      <c r="D71" s="67"/>
+      <c r="C71" s="64"/>
+      <c r="D71" s="65"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="49" t="s">
+      <c r="A72" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B72" s="65" t="s">
+      <c r="B72" s="63" t="s">
         <v>179</v>
       </c>
-      <c r="C72" s="66"/>
-      <c r="D72" s="67"/>
+      <c r="C72" s="64"/>
+      <c r="D72" s="65"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="49" t="s">
+      <c r="A73" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="B73" s="65" t="s">
+      <c r="B73" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="C73" s="66"/>
-      <c r="D73" s="67"/>
+      <c r="C73" s="64"/>
+      <c r="D73" s="65"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="49" t="s">
+      <c r="A74" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B74" s="65" t="s">
+      <c r="B74" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="66"/>
-      <c r="D74" s="67"/>
+      <c r="C74" s="64"/>
+      <c r="D74" s="65"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="49" t="s">
+      <c r="A75" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B75" s="65" t="s">
+      <c r="B75" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="C75" s="66"/>
-      <c r="D75" s="67"/>
+      <c r="C75" s="64"/>
+      <c r="D75" s="65"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="49" t="s">
+      <c r="A76" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="B76" s="65" t="s">
+      <c r="B76" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="C76" s="66"/>
-      <c r="D76" s="67"/>
+      <c r="C76" s="64"/>
+      <c r="D76" s="65"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="49" t="s">
+      <c r="A77" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B77" s="65" t="s">
+      <c r="B77" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="C77" s="66"/>
-      <c r="D77" s="67"/>
+      <c r="C77" s="64"/>
+      <c r="D77" s="65"/>
     </row>
     <row r="78" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="49" t="s">
+      <c r="A78" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="B78" s="65" t="s">
+      <c r="B78" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="C78" s="66"/>
-      <c r="D78" s="67"/>
+      <c r="C78" s="64"/>
+      <c r="D78" s="65"/>
     </row>
     <row r="79" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="49" t="s">
+      <c r="A79" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B79" s="65" t="s">
+      <c r="B79" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="C79" s="66"/>
-      <c r="D79" s="67"/>
+      <c r="C79" s="64"/>
+      <c r="D79" s="65"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="49" t="s">
+      <c r="A80" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="65" t="s">
+      <c r="B80" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="C80" s="66"/>
-      <c r="D80" s="67"/>
+      <c r="C80" s="64"/>
+      <c r="D80" s="65"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="49" t="s">
+      <c r="A81" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="B81" s="65" t="s">
+      <c r="B81" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="C81" s="66"/>
-      <c r="D81" s="67"/>
+      <c r="C81" s="64"/>
+      <c r="D81" s="65"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="49" t="s">
+      <c r="A82" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B82" s="65" t="s">
+      <c r="B82" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="C82" s="66"/>
-      <c r="D82" s="67"/>
+      <c r="C82" s="64"/>
+      <c r="D82" s="65"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="49" t="s">
+      <c r="A83" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B83" s="65" t="s">
+      <c r="B83" s="63" t="s">
+        <v>194</v>
+      </c>
+      <c r="C83" s="64"/>
+      <c r="D83" s="65"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="47" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="C84" s="57"/>
+      <c r="D84" s="58"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85" s="63" t="s">
+        <v>187</v>
+      </c>
+      <c r="C85" s="64"/>
+      <c r="D85" s="65"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="47" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86" s="63" t="s">
+        <v>107</v>
+      </c>
+      <c r="C86" s="64"/>
+      <c r="D86" s="65"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="47" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="C87" s="34"/>
+      <c r="D87" s="48"/>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="B88" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="C88" s="16"/>
+      <c r="D88" s="48"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="47" t="s">
+        <v>108</v>
+      </c>
+      <c r="B89" s="63" t="s">
+        <v>105</v>
+      </c>
+      <c r="C89" s="64"/>
+      <c r="D89" s="65"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="47" t="s">
+        <v>115</v>
+      </c>
+      <c r="B90" s="63" t="s">
+        <v>117</v>
+      </c>
+      <c r="C90" s="64"/>
+      <c r="D90" s="65"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="B91" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="C91" s="64"/>
+      <c r="D91" s="65"/>
+    </row>
+    <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="47" t="s">
         <v>185</v>
       </c>
-      <c r="C83" s="66"/>
-      <c r="D83" s="67"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="49" t="s">
-        <v>92</v>
-      </c>
-      <c r="B84" s="58" t="s">
-        <v>184</v>
-      </c>
-      <c r="C84" s="59"/>
-      <c r="D84" s="60"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="49" t="s">
-        <v>96</v>
-      </c>
-      <c r="B85" s="65" t="s">
-        <v>188</v>
-      </c>
-      <c r="C85" s="66"/>
-      <c r="D85" s="67"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="B86" s="65" t="s">
-        <v>107</v>
-      </c>
-      <c r="C86" s="66"/>
-      <c r="D86" s="67"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="49" t="s">
-        <v>98</v>
-      </c>
-      <c r="B87" s="35" t="s">
-        <v>109</v>
-      </c>
-      <c r="C87" s="36"/>
-      <c r="D87" s="50"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="49" t="s">
-        <v>106</v>
-      </c>
-      <c r="B88" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="C88" s="16"/>
-      <c r="D88" s="50"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="B89" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="C89" s="66"/>
-      <c r="D89" s="67"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="49" t="s">
-        <v>115</v>
-      </c>
-      <c r="B90" s="65" t="s">
-        <v>117</v>
-      </c>
-      <c r="C90" s="66"/>
-      <c r="D90" s="67"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="49" t="s">
-        <v>147</v>
-      </c>
-      <c r="B91" s="65" t="s">
-        <v>116</v>
-      </c>
-      <c r="C91" s="66"/>
-      <c r="D91" s="67"/>
-    </row>
-    <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="49" t="s">
-        <v>186</v>
-      </c>
-      <c r="B92" s="62" t="s">
+      <c r="B92" s="112" t="s">
         <v>156</v>
       </c>
-      <c r="C92" s="63"/>
-      <c r="D92" s="64"/>
+      <c r="C92" s="113"/>
+      <c r="D92" s="114"/>
     </row>
   </sheetData>
   <mergeCells count="63">
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="B86:D86"/>
+    <mergeCell ref="B89:D89"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="D37:D40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="B42:B44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="A48:D48"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="A60:D60"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="A64:D64"/>
+    <mergeCell ref="A69:D69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="A4:A11"/>
+    <mergeCell ref="B4:B11"/>
+    <mergeCell ref="D4:D11"/>
+    <mergeCell ref="B65:C65"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="B15:B17"/>
+    <mergeCell ref="A19:D19"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="D25:D29"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="A34:A35"/>
+    <mergeCell ref="D34:D35"/>
     <mergeCell ref="B81:D81"/>
     <mergeCell ref="B82:D82"/>
     <mergeCell ref="B83:D83"/>
@@ -3070,53 +3126,6 @@
     <mergeCell ref="B74:D74"/>
     <mergeCell ref="B73:D73"/>
     <mergeCell ref="A25:A26"/>
-    <mergeCell ref="B65:C65"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="A19:D19"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="D25:D29"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="A31:D31"/>
-    <mergeCell ref="D32:D33"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="D34:D35"/>
-    <mergeCell ref="A60:D60"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="A64:D64"/>
-    <mergeCell ref="A69:D69"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="A4:A11"/>
-    <mergeCell ref="B4:B11"/>
-    <mergeCell ref="D4:D11"/>
-    <mergeCell ref="B47:D47"/>
-    <mergeCell ref="A48:D48"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B37:B40"/>
-    <mergeCell ref="D37:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="B42:B44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="B86:D86"/>
-    <mergeCell ref="B89:D89"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="B91:D91"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
added all TC 6 update, delete, fixed search method
</commit_message>
<xml_diff>
--- a/doc/TA.Final.TestCases.DoroshenkoDenis.xlsx
+++ b/doc/TA.Final.TestCases.DoroshenkoDenis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\NetcrackerLearningCenter\finalPractice\cucumber-selenium\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8A23E85-5D86-4774-8101-CD8D665CAB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC27B5CA-69DD-4058-94AB-24CEEFBA6F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="-8010" windowWidth="16440" windowHeight="28440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -521,12 +521,6 @@
 …</t>
   </si>
   <si>
-    <t>Delete Device parameters</t>
-  </si>
-  <si>
-    <t>Name: "test_city_delete"; Population: 999999</t>
-  </si>
-  <si>
     <t>1. Repeat steps from TC_5.1
 2. Click "Create country", Fill fields with test data1 and Click "Save"
 3. Click "Cities" and "Create city", Fill fields with test data11 and Click "Save"
@@ -675,6 +669,12 @@
   </si>
   <si>
     <t>Name: "Torre InterPlaza"; Street Name: "Boulevard Juan Pablo"; Is connected: Lit</t>
+  </si>
+  <si>
+    <t>Delete object</t>
+  </si>
+  <si>
+    <t>Name: "San Pedro Sula"; Population: 489466</t>
   </si>
 </sst>
 </file>
@@ -776,7 +776,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1393,7 +1393,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="120">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1571,10 +1571,16 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="38" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1722,6 +1728,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="47" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2077,8 +2092,8 @@
   </sheetPr>
   <dimension ref="A1:F92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B92" sqref="B92:D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2109,12 +2124,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="92" t="s">
+      <c r="A2" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="93"/>
-      <c r="C2" s="93"/>
-      <c r="D2" s="94"/>
+      <c r="B2" s="95"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="96"/>
       <c r="F2" s="6" t="s">
         <v>20</v>
       </c>
@@ -2123,82 +2138,82 @@
       <c r="A3" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="110" t="s">
         <v>88</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="109"/>
+      <c r="C3" s="110"/>
+      <c r="D3" s="111"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="110" t="s">
+      <c r="A4" s="112" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="84" t="s">
+      <c r="B4" s="86" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="111" t="s">
+      <c r="D4" s="113" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="110"/>
-      <c r="B5" s="84"/>
+      <c r="A5" s="112"/>
+      <c r="B5" s="86"/>
       <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D5" s="111"/>
+      <c r="D5" s="113"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="110"/>
-      <c r="B6" s="84"/>
+      <c r="A6" s="112"/>
+      <c r="B6" s="86"/>
       <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="111"/>
+      <c r="D6" s="113"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="110"/>
-      <c r="B7" s="84"/>
+      <c r="A7" s="112"/>
+      <c r="B7" s="86"/>
       <c r="C7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="111"/>
+      <c r="D7" s="113"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="110"/>
-      <c r="B8" s="84"/>
+      <c r="A8" s="112"/>
+      <c r="B8" s="86"/>
       <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="111"/>
+      <c r="D8" s="113"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="110"/>
-      <c r="B9" s="84"/>
+      <c r="A9" s="112"/>
+      <c r="B9" s="86"/>
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="111"/>
+      <c r="D9" s="113"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="110"/>
-      <c r="B10" s="84"/>
+      <c r="A10" s="112"/>
+      <c r="B10" s="86"/>
       <c r="C10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="111"/>
+      <c r="D10" s="113"/>
       <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="110"/>
-      <c r="B11" s="84"/>
+      <c r="A11" s="112"/>
+      <c r="B11" s="86"/>
       <c r="C11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="111"/>
+      <c r="D11" s="113"/>
     </row>
     <row r="12" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="49" t="s">
@@ -2232,81 +2247,81 @@
       <c r="A14" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="66" t="s">
+      <c r="B14" s="68" t="s">
         <v>45</v>
       </c>
-      <c r="C14" s="67"/>
-      <c r="D14" s="68"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="70"/>
     </row>
     <row r="15" spans="1:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="78" t="s">
+      <c r="A15" s="80" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="81" t="s">
-        <v>158</v>
+      <c r="B15" s="83" t="s">
+        <v>156</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="69" t="s">
+      <c r="D15" s="71" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="79"/>
-      <c r="B16" s="82"/>
+      <c r="A16" s="81"/>
+      <c r="B16" s="84"/>
       <c r="C16" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="D16" s="70"/>
+        <v>157</v>
+      </c>
+      <c r="D16" s="72"/>
     </row>
     <row r="17" spans="1:4" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="80"/>
-      <c r="B17" s="83"/>
+      <c r="A17" s="82"/>
+      <c r="B17" s="85"/>
       <c r="C17" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="71"/>
+      <c r="D17" s="73"/>
     </row>
     <row r="18" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="66" t="s">
+      <c r="B18" s="68" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="67"/>
-      <c r="D18" s="68"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="70"/>
     </row>
     <row r="19" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="72" t="s">
+      <c r="A19" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="74"/>
+      <c r="B19" s="75"/>
+      <c r="C19" s="75"/>
+      <c r="D19" s="76"/>
     </row>
     <row r="20" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="77" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="84" t="s">
+      <c r="B20" s="86" t="s">
         <v>80</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D20" s="69" t="s">
+      <c r="D20" s="71" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="75"/>
-      <c r="B21" s="84"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="86"/>
       <c r="C21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="70"/>
+      <c r="D21" s="72"/>
     </row>
     <row r="22" spans="1:4" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="51" t="s">
@@ -2318,47 +2333,47 @@
       <c r="C22" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D22" s="71"/>
+      <c r="D22" s="73"/>
     </row>
     <row r="23" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="66" t="s">
+      <c r="B23" s="68" t="s">
         <v>57</v>
       </c>
-      <c r="C23" s="67"/>
-      <c r="D23" s="68"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="70"/>
     </row>
     <row r="24" spans="1:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="72" t="s">
+      <c r="A24" s="74" t="s">
         <v>60</v>
       </c>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="74"/>
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="76"/>
     </row>
     <row r="25" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="75" t="s">
+      <c r="A25" s="77" t="s">
         <v>61</v>
       </c>
-      <c r="B25" s="84" t="s">
+      <c r="B25" s="86" t="s">
         <v>75</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D25" s="69" t="s">
+        <v>174</v>
+      </c>
+      <c r="D25" s="71" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="75"/>
-      <c r="B26" s="84"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="86"/>
       <c r="C26" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="70"/>
+      <c r="D26" s="72"/>
     </row>
     <row r="27" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="53" t="s">
@@ -2370,7 +2385,7 @@
       <c r="C27" s="23" t="s">
         <v>65</v>
       </c>
-      <c r="D27" s="70"/>
+      <c r="D27" s="72"/>
     </row>
     <row r="28" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="52" t="s">
@@ -2382,7 +2397,7 @@
       <c r="C28" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D28" s="70"/>
+      <c r="D28" s="72"/>
     </row>
     <row r="29" spans="1:4" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="54" t="s">
@@ -2394,69 +2409,69 @@
       <c r="C29" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="D29" s="71"/>
+      <c r="D29" s="73"/>
     </row>
     <row r="30" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="B30" s="66" t="s">
+      <c r="B30" s="68" t="s">
         <v>124</v>
       </c>
-      <c r="C30" s="67"/>
-      <c r="D30" s="68"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="70"/>
     </row>
     <row r="31" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="85" t="s">
-        <v>161</v>
-      </c>
-      <c r="B31" s="86"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="87"/>
+      <c r="A31" s="87" t="s">
+        <v>159</v>
+      </c>
+      <c r="B31" s="88"/>
+      <c r="C31" s="88"/>
+      <c r="D31" s="89"/>
     </row>
     <row r="32" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="90" t="s">
+      <c r="A32" s="92" t="s">
         <v>74</v>
       </c>
-      <c r="B32" s="81" t="s">
+      <c r="B32" s="83" t="s">
         <v>84</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D32" s="69" t="s">
+      <c r="D32" s="71" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="91"/>
-      <c r="B33" s="89"/>
+      <c r="A33" s="93"/>
+      <c r="B33" s="91"/>
       <c r="C33" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="D33" s="88"/>
+      <c r="D33" s="90"/>
     </row>
     <row r="34" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="92" t="s">
         <v>83</v>
       </c>
-      <c r="B34" s="81" t="s">
+      <c r="B34" s="83" t="s">
         <v>85</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D34" s="69" t="s">
+      <c r="D34" s="71" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="91"/>
-      <c r="B35" s="89"/>
+      <c r="A35" s="93"/>
+      <c r="B35" s="91"/>
       <c r="C35" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="D35" s="88"/>
+        <v>179</v>
+      </c>
+      <c r="D35" s="90"/>
     </row>
     <row r="36" spans="1:4" ht="162" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="55" t="s">
@@ -2466,7 +2481,7 @@
         <v>94</v>
       </c>
       <c r="C36" s="25" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D36" s="22" t="s">
         <v>99</v>
@@ -2476,65 +2491,65 @@
       <c r="A37" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="B37" s="81" t="s">
+      <c r="B37" s="83" t="s">
         <v>113</v>
       </c>
       <c r="C37" s="25" t="s">
-        <v>188</v>
-      </c>
-      <c r="D37" s="69" t="s">
-        <v>193</v>
+        <v>186</v>
+      </c>
+      <c r="D37" s="71" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="59" t="s">
         <v>111</v>
       </c>
-      <c r="B38" s="82"/>
+      <c r="B38" s="84"/>
       <c r="C38" s="25" t="s">
-        <v>189</v>
-      </c>
-      <c r="D38" s="70"/>
+        <v>187</v>
+      </c>
+      <c r="D38" s="72"/>
     </row>
     <row r="39" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="B39" s="82"/>
+      <c r="B39" s="84"/>
       <c r="C39" s="25" t="s">
-        <v>190</v>
-      </c>
-      <c r="D39" s="70"/>
+        <v>188</v>
+      </c>
+      <c r="D39" s="72"/>
     </row>
     <row r="40" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="B40" s="89"/>
+      <c r="B40" s="91"/>
       <c r="C40" s="25" t="s">
-        <v>191</v>
-      </c>
-      <c r="D40" s="88"/>
+        <v>189</v>
+      </c>
+      <c r="D40" s="90"/>
     </row>
     <row r="41" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="85" t="s">
+      <c r="A41" s="87" t="s">
         <v>118</v>
       </c>
-      <c r="B41" s="86"/>
-      <c r="C41" s="86"/>
-      <c r="D41" s="87"/>
+      <c r="B41" s="88"/>
+      <c r="C41" s="88"/>
+      <c r="D41" s="89"/>
     </row>
     <row r="42" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="60" t="s">
         <v>119</v>
       </c>
-      <c r="B42" s="81" t="s">
+      <c r="B42" s="114" t="s">
         <v>154</v>
       </c>
       <c r="C42" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="D42" s="69" t="s">
+      <c r="D42" s="71" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2542,24 +2557,24 @@
       <c r="A43" s="60" t="s">
         <v>153</v>
       </c>
-      <c r="B43" s="82"/>
+      <c r="B43" s="115"/>
       <c r="C43" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="70"/>
+      <c r="D43" s="72"/>
     </row>
     <row r="44" spans="1:4" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="60" t="s">
         <v>152</v>
       </c>
-      <c r="B44" s="89"/>
+      <c r="B44" s="116"/>
       <c r="C44" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="D44" s="88"/>
+      <c r="D44" s="90"/>
     </row>
     <row r="45" spans="1:4" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="62" t="s">
+      <c r="A45" s="61" t="s">
         <v>95</v>
       </c>
       <c r="B45" s="27" t="s">
@@ -2590,25 +2605,25 @@
       <c r="A47" s="21" t="s">
         <v>123</v>
       </c>
-      <c r="B47" s="66" t="s">
+      <c r="B47" s="68" t="s">
         <v>125</v>
       </c>
-      <c r="C47" s="67"/>
-      <c r="D47" s="68"/>
+      <c r="C47" s="69"/>
+      <c r="D47" s="70"/>
     </row>
     <row r="48" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="85" t="s">
-        <v>162</v>
-      </c>
-      <c r="B48" s="86"/>
-      <c r="C48" s="86"/>
-      <c r="D48" s="87"/>
+      <c r="A48" s="87" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48" s="88"/>
+      <c r="C48" s="88"/>
+      <c r="D48" s="89"/>
     </row>
     <row r="49" spans="1:4" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="62" t="s">
         <v>140</v>
       </c>
       <c r="C49" s="26" t="s">
@@ -2636,7 +2651,7 @@
       <c r="A51" s="18" t="s">
         <v>128</v>
       </c>
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="64" t="s">
         <v>146</v>
       </c>
       <c r="C51" s="26" t="s">
@@ -2650,23 +2665,23 @@
       <c r="A52" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="B52" s="29" t="s">
+      <c r="B52" s="64" t="s">
+        <v>193</v>
+      </c>
+      <c r="C52" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="C52" s="26" t="s">
-        <v>157</v>
-      </c>
       <c r="D52" s="14"/>
     </row>
     <row r="53" spans="1:4" ht="76.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="61" t="s">
+      <c r="A53" s="63" t="s">
         <v>130</v>
       </c>
       <c r="B53" s="29" t="s">
+        <v>156</v>
+      </c>
+      <c r="C53" s="26" t="s">
         <v>158</v>
-      </c>
-      <c r="C53" s="26" t="s">
-        <v>160</v>
       </c>
       <c r="D53" s="14" t="s">
         <v>48</v>
@@ -2676,32 +2691,32 @@
       <c r="A54" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="B54" s="66" t="s">
+      <c r="B54" s="68" t="s">
         <v>131</v>
       </c>
-      <c r="C54" s="67"/>
-      <c r="D54" s="68"/>
+      <c r="C54" s="69"/>
+      <c r="D54" s="70"/>
     </row>
     <row r="55" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="85" t="s">
-        <v>164</v>
-      </c>
-      <c r="B55" s="86"/>
-      <c r="C55" s="86"/>
-      <c r="D55" s="87"/>
+      <c r="A55" s="87" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" s="88"/>
+      <c r="C55" s="88"/>
+      <c r="D55" s="89"/>
     </row>
     <row r="56" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18" t="s">
         <v>133</v>
       </c>
       <c r="B56" s="29" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" s="26" t="s">
         <v>166</v>
       </c>
-      <c r="C56" s="26" t="s">
-        <v>168</v>
-      </c>
       <c r="D56" s="14" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2709,13 +2724,13 @@
         <v>134</v>
       </c>
       <c r="B57" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="C57" s="26" t="s">
         <v>167</v>
       </c>
-      <c r="C57" s="26" t="s">
+      <c r="D57" s="14" t="s">
         <v>169</v>
-      </c>
-      <c r="D57" s="14" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2723,42 +2738,42 @@
         <v>135</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C58" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="D58" s="14" t="s">
         <v>170</v>
-      </c>
-      <c r="D58" s="14" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="B59" s="66" t="s">
+      <c r="B59" s="68" t="s">
         <v>136</v>
       </c>
-      <c r="C59" s="67"/>
-      <c r="D59" s="68"/>
+      <c r="C59" s="69"/>
+      <c r="D59" s="70"/>
     </row>
     <row r="60" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="85" t="s">
-        <v>163</v>
-      </c>
-      <c r="B60" s="86"/>
-      <c r="C60" s="86"/>
-      <c r="D60" s="87"/>
+      <c r="A60" s="87" t="s">
+        <v>161</v>
+      </c>
+      <c r="B60" s="88"/>
+      <c r="C60" s="88"/>
+      <c r="D60" s="89"/>
     </row>
     <row r="61" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18" t="s">
         <v>138</v>
       </c>
       <c r="B61" s="41" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C61" s="26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D61" s="14" t="s">
         <v>29</v>
@@ -2769,48 +2784,48 @@
         <v>139</v>
       </c>
       <c r="B62" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="C62" s="36" t="s">
         <v>173</v>
-      </c>
-      <c r="C62" s="36" t="s">
-        <v>175</v>
       </c>
       <c r="D62" s="38" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="107"/>
-      <c r="B63" s="107"/>
-      <c r="C63" s="107"/>
-      <c r="D63" s="107"/>
+      <c r="A63" s="109"/>
+      <c r="B63" s="109"/>
+      <c r="C63" s="109"/>
+      <c r="D63" s="109"/>
     </row>
     <row r="64" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="95" t="s">
+      <c r="A64" s="97" t="s">
         <v>7</v>
       </c>
-      <c r="B64" s="96"/>
-      <c r="C64" s="96"/>
-      <c r="D64" s="97"/>
+      <c r="B64" s="98"/>
+      <c r="C64" s="98"/>
+      <c r="D64" s="99"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="B65" s="76" t="s">
+      <c r="B65" s="78" t="s">
         <v>49</v>
       </c>
-      <c r="C65" s="77"/>
+      <c r="C65" s="79"/>
       <c r="D65" s="40"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="B66" s="104" t="s">
+      <c r="B66" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="C66" s="105"/>
-      <c r="D66" s="106"/>
+      <c r="C66" s="107"/>
+      <c r="D66" s="108"/>
     </row>
     <row r="67" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="43" t="s">
@@ -2824,159 +2839,159 @@
     </row>
     <row r="68" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="69" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A69" s="98" t="s">
+      <c r="A69" s="100" t="s">
         <v>5</v>
       </c>
-      <c r="B69" s="99"/>
-      <c r="C69" s="99"/>
-      <c r="D69" s="100"/>
+      <c r="B69" s="101"/>
+      <c r="C69" s="101"/>
+      <c r="D69" s="102"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="47" t="s">
         <v>9</v>
       </c>
-      <c r="B70" s="101" t="s">
-        <v>177</v>
-      </c>
-      <c r="C70" s="102"/>
-      <c r="D70" s="103"/>
+      <c r="B70" s="103" t="s">
+        <v>175</v>
+      </c>
+      <c r="C70" s="104"/>
+      <c r="D70" s="105"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="47" t="s">
         <v>10</v>
       </c>
-      <c r="B71" s="63" t="s">
-        <v>178</v>
-      </c>
-      <c r="C71" s="64"/>
-      <c r="D71" s="65"/>
+      <c r="B71" s="65" t="s">
+        <v>176</v>
+      </c>
+      <c r="C71" s="66"/>
+      <c r="D71" s="67"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="47" t="s">
         <v>33</v>
       </c>
-      <c r="B72" s="63" t="s">
-        <v>179</v>
-      </c>
-      <c r="C72" s="64"/>
-      <c r="D72" s="65"/>
+      <c r="B72" s="65" t="s">
+        <v>177</v>
+      </c>
+      <c r="C72" s="66"/>
+      <c r="D72" s="67"/>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="B73" s="63" t="s">
+      <c r="B73" s="65" t="s">
         <v>68</v>
       </c>
-      <c r="C73" s="64"/>
-      <c r="D73" s="65"/>
+      <c r="C73" s="66"/>
+      <c r="D73" s="67"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="47" t="s">
         <v>34</v>
       </c>
-      <c r="B74" s="63" t="s">
+      <c r="B74" s="65" t="s">
         <v>69</v>
       </c>
-      <c r="C74" s="64"/>
-      <c r="D74" s="65"/>
+      <c r="C74" s="66"/>
+      <c r="D74" s="67"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="47" t="s">
         <v>39</v>
       </c>
-      <c r="B75" s="63" t="s">
+      <c r="B75" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="C75" s="64"/>
-      <c r="D75" s="65"/>
+      <c r="C75" s="66"/>
+      <c r="D75" s="67"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="47" t="s">
         <v>35</v>
       </c>
-      <c r="B76" s="63" t="s">
-        <v>180</v>
-      </c>
-      <c r="C76" s="64"/>
-      <c r="D76" s="65"/>
+      <c r="B76" s="65" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76" s="66"/>
+      <c r="D76" s="67"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="47" t="s">
         <v>40</v>
       </c>
-      <c r="B77" s="63" t="s">
+      <c r="B77" s="65" t="s">
         <v>71</v>
       </c>
-      <c r="C77" s="64"/>
-      <c r="D77" s="65"/>
+      <c r="C77" s="66"/>
+      <c r="D77" s="67"/>
     </row>
     <row r="78" spans="1:4" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="47" t="s">
         <v>36</v>
       </c>
-      <c r="B78" s="63" t="s">
+      <c r="B78" s="65" t="s">
         <v>72</v>
       </c>
-      <c r="C78" s="64"/>
-      <c r="D78" s="65"/>
+      <c r="C78" s="66"/>
+      <c r="D78" s="67"/>
     </row>
     <row r="79" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="47" t="s">
         <v>11</v>
       </c>
-      <c r="B79" s="63" t="s">
+      <c r="B79" s="65" t="s">
         <v>148</v>
       </c>
-      <c r="C79" s="64"/>
-      <c r="D79" s="65"/>
+      <c r="C79" s="66"/>
+      <c r="D79" s="67"/>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="47" t="s">
         <v>37</v>
       </c>
-      <c r="B80" s="63" t="s">
+      <c r="B80" s="65" t="s">
         <v>149</v>
       </c>
-      <c r="C80" s="64"/>
-      <c r="D80" s="65"/>
+      <c r="C80" s="66"/>
+      <c r="D80" s="67"/>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="47" t="s">
         <v>89</v>
       </c>
-      <c r="B81" s="63" t="s">
-        <v>182</v>
-      </c>
-      <c r="C81" s="64"/>
-      <c r="D81" s="65"/>
+      <c r="B81" s="65" t="s">
+        <v>180</v>
+      </c>
+      <c r="C81" s="66"/>
+      <c r="D81" s="67"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="B82" s="63" t="s">
-        <v>183</v>
-      </c>
-      <c r="C82" s="64"/>
-      <c r="D82" s="65"/>
+      <c r="B82" s="65" t="s">
+        <v>181</v>
+      </c>
+      <c r="C82" s="66"/>
+      <c r="D82" s="67"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="47" t="s">
         <v>91</v>
       </c>
-      <c r="B83" s="63" t="s">
-        <v>194</v>
-      </c>
-      <c r="C83" s="64"/>
-      <c r="D83" s="65"/>
+      <c r="B83" s="65" t="s">
+        <v>192</v>
+      </c>
+      <c r="C83" s="66"/>
+      <c r="D83" s="67"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="47" t="s">
         <v>92</v>
       </c>
       <c r="B84" s="56" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C84" s="57"/>
       <c r="D84" s="58"/>
@@ -2985,21 +3000,21 @@
       <c r="A85" s="47" t="s">
         <v>96</v>
       </c>
-      <c r="B85" s="63" t="s">
-        <v>187</v>
-      </c>
-      <c r="C85" s="64"/>
-      <c r="D85" s="65"/>
+      <c r="B85" s="65" t="s">
+        <v>185</v>
+      </c>
+      <c r="C85" s="66"/>
+      <c r="D85" s="67"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="47" t="s">
         <v>97</v>
       </c>
-      <c r="B86" s="63" t="s">
+      <c r="B86" s="65" t="s">
         <v>107</v>
       </c>
-      <c r="C86" s="64"/>
-      <c r="D86" s="65"/>
+      <c r="C86" s="66"/>
+      <c r="D86" s="67"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="47" t="s">
@@ -3016,7 +3031,7 @@
         <v>106</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C88" s="16"/>
       <c r="D88" s="48"/>
@@ -3025,41 +3040,41 @@
       <c r="A89" s="47" t="s">
         <v>108</v>
       </c>
-      <c r="B89" s="63" t="s">
+      <c r="B89" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="C89" s="64"/>
-      <c r="D89" s="65"/>
+      <c r="C89" s="66"/>
+      <c r="D89" s="67"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="B90" s="63" t="s">
+      <c r="B90" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="C90" s="64"/>
-      <c r="D90" s="65"/>
+      <c r="C90" s="66"/>
+      <c r="D90" s="67"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="B91" s="63" t="s">
+      <c r="B91" s="65" t="s">
         <v>116</v>
       </c>
-      <c r="C91" s="64"/>
-      <c r="D91" s="65"/>
+      <c r="C91" s="66"/>
+      <c r="D91" s="67"/>
     </row>
     <row r="92" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="47" t="s">
-        <v>185</v>
-      </c>
-      <c r="B92" s="112" t="s">
-        <v>156</v>
-      </c>
-      <c r="C92" s="113"/>
-      <c r="D92" s="114"/>
+        <v>183</v>
+      </c>
+      <c r="B92" s="117" t="s">
+        <v>194</v>
+      </c>
+      <c r="C92" s="118"/>
+      <c r="D92" s="119"/>
     </row>
   </sheetData>
   <mergeCells count="63">

</xml_diff>